<commit_message>
Figured out Part 1, partially
</commit_message>
<xml_diff>
--- a/Network Example/Example_Tables.xlsx
+++ b/Network Example/Example_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\td830f\Documents\Projects\MBSec\AAR Feature\_PowerBI Version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F894A5-6802-4B7A-98C0-E38F78C6F66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF72D2C-D0BA-40E8-9001-153D182C8F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{358D1994-51E7-4B4D-80E1-29ED415900C3}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>Data Exchange ID</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>OE Sort Order</t>
+  </si>
+  <si>
+    <t>Node Parent ID</t>
   </si>
 </sst>
 </file>
@@ -561,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEF5C72-248A-4464-BBEB-45DF6BB0594E}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="D9" sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,9 +575,10 @@
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -584,8 +588,11 @@
       <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -595,8 +602,9 @@
       <c r="C2" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -606,8 +614,11 @@
       <c r="C3" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -617,8 +628,11 @@
       <c r="C4" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -628,8 +642,9 @@
       <c r="C5" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -639,8 +654,11 @@
       <c r="C6" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -650,8 +668,11 @@
       <c r="C7" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -661,8 +682,11 @@
       <c r="C8" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -672,6 +696,7 @@
       <c r="C9" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1006,7 +1031,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1157,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B1" sqref="B1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>